<commit_message>
Added folder and modified files
</commit_message>
<xml_diff>
--- a/data/raw/Crime_statistics_2023V1.xlsx
+++ b/data/raw/Crime_statistics_2023V1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\ironhack\Week_5\Mid_bootcamp_project\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PIVOT" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="115">
   <si>
     <t>:</t>
   </si>
@@ -519,11 +519,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0_i"/>
     <numFmt numFmtId="167" formatCode="#,##0_i"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -855,7 +856,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -1107,10 +1108,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal 2" xfId="3"/>
@@ -6223,7 +6226,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6319,7 +6321,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -25145,10 +25146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25172,64 +25173,64 @@
     <col min="17" max="17" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="118" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+    <row r="1" spans="1:17" s="117" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="117" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="118" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
+    <row r="2" spans="1:17" s="117" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="118" t="s">
+      <c r="C2" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="118" t="s">
+      <c r="D2" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="118" t="s">
+      <c r="E2" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="118" t="s">
+      <c r="F2" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="118" t="s">
+      <c r="G2" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="118" t="s">
+      <c r="H2" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="118" t="s">
+      <c r="I2" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="118" t="s">
+      <c r="J2" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="118" t="s">
+      <c r="K2" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="118" t="s">
+      <c r="L2" s="117" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="118" t="s">
+      <c r="M2" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="118" t="s">
+      <c r="N2" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="118" t="s">
+      <c r="O2" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="118" t="s">
+      <c r="P2" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="118" t="s">
+      <c r="Q2" s="117" t="s">
         <v>42</v>
       </c>
     </row>
@@ -25818,903 +25819,1281 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B14">
-        <v>23532.449999999993</v>
+        <v>551.91999999999996</v>
       </c>
       <c r="C14">
-        <v>10656.269999999999</v>
+        <v>37.869999999999997</v>
       </c>
       <c r="D14">
-        <v>6577.72</v>
+        <v>112.17</v>
       </c>
       <c r="E14">
-        <v>5841.1400000000012</v>
+        <v>125.14</v>
       </c>
       <c r="F14">
-        <v>1966.58</v>
+        <v>11.11</v>
       </c>
       <c r="G14">
-        <v>1108.6700000000003</v>
+        <v>3</v>
       </c>
       <c r="H14">
-        <v>919.07999999999993</v>
+        <v>22.5</v>
       </c>
       <c r="I14">
-        <v>705.09999999999991</v>
+        <v>3.62</v>
       </c>
       <c r="J14">
-        <v>694.58</v>
+        <v>7.09</v>
       </c>
       <c r="K14">
-        <v>344.53999999999996</v>
+        <v>1.07</v>
       </c>
       <c r="L14">
-        <v>264.44</v>
+        <v>0.32</v>
       </c>
       <c r="M14">
-        <v>63.059999999999995</v>
+        <v>1.42</v>
       </c>
       <c r="N14">
-        <v>34.850000000000009</v>
+        <v>3.35</v>
       </c>
       <c r="O14">
-        <v>28.97</v>
+        <v>0.83</v>
       </c>
       <c r="P14">
-        <v>24.840000000000003</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="Q14">
-        <v>52762.290000000008</v>
+        <v>881.99</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>551.91999999999996</v>
+        <v>436.02</v>
       </c>
       <c r="C15">
-        <v>37.869999999999997</v>
+        <v>158.16</v>
       </c>
       <c r="D15">
-        <v>112.17</v>
+        <v>71.64</v>
       </c>
       <c r="E15">
-        <v>125.14</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>11.11</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="H15">
-        <v>22.5</v>
+        <v>5.56</v>
       </c>
       <c r="I15">
-        <v>3.62</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>7.09</v>
+        <v>66.959999999999994</v>
       </c>
       <c r="K15">
-        <v>1.07</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="L15">
-        <v>0.32</v>
+        <v>3.08</v>
       </c>
       <c r="M15">
-        <v>1.42</v>
+        <v>0.65</v>
       </c>
       <c r="N15">
-        <v>3.35</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>0.83</v>
+        <v>0.69</v>
       </c>
       <c r="P15">
-        <v>0.57999999999999996</v>
+        <v>0.04</v>
       </c>
       <c r="Q15">
-        <v>881.99</v>
+        <v>752.76</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B16">
-        <v>436.02</v>
+        <v>891.23</v>
       </c>
       <c r="C16">
-        <v>158.16</v>
+        <v>118.08</v>
       </c>
       <c r="D16">
-        <v>71.64</v>
+        <v>384.39</v>
       </c>
       <c r="E16">
+        <v>167.51</v>
+      </c>
+      <c r="F16">
+        <v>96.24</v>
+      </c>
+      <c r="G16">
+        <v>58.35</v>
+      </c>
+      <c r="H16">
+        <v>23.43</v>
+      </c>
+      <c r="I16">
+        <v>2.14</v>
+      </c>
+      <c r="J16">
+        <v>0.16</v>
+      </c>
+      <c r="K16">
+        <v>10.23</v>
+      </c>
+      <c r="L16">
         <v>0</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="H16">
-        <v>5.56</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>66.959999999999994</v>
-      </c>
-      <c r="K16">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="L16">
-        <v>3.08</v>
-      </c>
       <c r="M16">
-        <v>0.65</v>
+        <v>0.32</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0.69</v>
+        <v>0.44</v>
       </c>
       <c r="P16">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="Q16">
-        <v>752.76</v>
+        <v>1754.52</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>891.23</v>
+        <v>1183.42</v>
       </c>
       <c r="C17">
-        <v>118.08</v>
+        <v>475.65</v>
       </c>
       <c r="D17">
-        <v>384.39</v>
+        <v>50.42</v>
       </c>
       <c r="E17">
-        <v>167.51</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>96.24</v>
+        <v>100.72</v>
       </c>
       <c r="G17">
-        <v>58.35</v>
+        <v>9.73</v>
       </c>
       <c r="H17">
-        <v>23.43</v>
+        <v>38.049999999999997</v>
       </c>
       <c r="I17">
-        <v>2.14</v>
+        <v>33.64</v>
       </c>
       <c r="J17">
-        <v>0.16</v>
+        <v>6.49</v>
       </c>
       <c r="K17">
-        <v>10.23</v>
+        <v>4.33</v>
       </c>
       <c r="L17">
+        <v>3.11</v>
+      </c>
+      <c r="M17">
         <v>0</v>
       </c>
-      <c r="M17">
-        <v>0.32</v>
-      </c>
       <c r="N17">
-        <v>0</v>
+        <v>1.19</v>
       </c>
       <c r="O17">
-        <v>0.44</v>
+        <v>0.51</v>
       </c>
       <c r="P17">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="Q17">
-        <v>1754.52</v>
+        <v>1907.4600000000003</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>1183.42</v>
+        <v>417.28</v>
       </c>
       <c r="C18">
-        <v>475.65</v>
+        <v>90.74</v>
       </c>
       <c r="D18">
-        <v>50.42</v>
+        <v>77.28</v>
       </c>
       <c r="E18">
+        <v>146.79</v>
+      </c>
+      <c r="F18">
+        <v>29</v>
+      </c>
+      <c r="G18">
+        <v>17.690000000000001</v>
+      </c>
+      <c r="H18">
+        <v>13.89</v>
+      </c>
+      <c r="I18">
+        <v>0.95</v>
+      </c>
+      <c r="J18">
+        <v>10.83</v>
+      </c>
+      <c r="K18">
+        <v>15.42</v>
+      </c>
+      <c r="L18">
+        <v>21.75</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>100.72</v>
-      </c>
-      <c r="G18">
-        <v>9.73</v>
-      </c>
-      <c r="H18">
-        <v>38.049999999999997</v>
-      </c>
-      <c r="I18">
-        <v>33.64</v>
-      </c>
-      <c r="J18">
-        <v>6.49</v>
-      </c>
-      <c r="K18">
-        <v>4.33</v>
-      </c>
-      <c r="L18">
-        <v>3.11</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>1.19</v>
-      </c>
       <c r="O18">
-        <v>0.51</v>
+        <v>5.18</v>
       </c>
       <c r="P18">
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
       <c r="Q18">
-        <v>1907.4600000000003</v>
+        <v>848.11999999999989</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>417.28</v>
+        <v>276.70999999999998</v>
       </c>
       <c r="C19">
-        <v>90.74</v>
+        <v>96.2</v>
       </c>
       <c r="D19">
-        <v>77.28</v>
+        <v>112.49</v>
       </c>
       <c r="E19">
-        <v>146.79</v>
+        <v>29.4</v>
       </c>
       <c r="F19">
-        <v>29</v>
+        <v>4.51</v>
       </c>
       <c r="G19">
-        <v>17.690000000000001</v>
+        <v>5.26</v>
       </c>
       <c r="H19">
-        <v>13.89</v>
+        <v>11.09</v>
       </c>
       <c r="I19">
-        <v>0.95</v>
+        <v>25.22</v>
       </c>
       <c r="J19">
-        <v>10.83</v>
+        <v>22.32</v>
       </c>
       <c r="K19">
-        <v>15.42</v>
+        <v>12.52</v>
       </c>
       <c r="L19">
-        <v>21.75</v>
+        <v>2.97</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0.21</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="O19">
-        <v>5.18</v>
+        <v>2.5</v>
       </c>
       <c r="P19">
-        <v>0.32</v>
+        <v>0.04</v>
       </c>
       <c r="Q19">
-        <v>848.11999999999989</v>
+        <v>601.61999999999989</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20">
-        <v>276.70999999999998</v>
+        <v>1717.58</v>
       </c>
       <c r="C20">
-        <v>96.2</v>
+        <v>235.58</v>
       </c>
       <c r="D20">
-        <v>112.49</v>
+        <v>594.42999999999995</v>
       </c>
       <c r="E20">
-        <v>29.4</v>
+        <v>489.34</v>
       </c>
       <c r="F20">
-        <v>4.51</v>
+        <v>86.34</v>
       </c>
       <c r="G20">
-        <v>5.26</v>
+        <v>54.83</v>
       </c>
       <c r="H20">
-        <v>11.09</v>
+        <v>93.74</v>
       </c>
       <c r="I20">
-        <v>25.22</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>22.32</v>
+        <v>0.63</v>
       </c>
       <c r="K20">
-        <v>12.52</v>
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>2.97</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>0.21</v>
+        <v>10.87</v>
       </c>
       <c r="N20">
-        <v>0.18</v>
+        <v>9.61</v>
       </c>
       <c r="O20">
-        <v>2.5</v>
+        <v>0.47</v>
       </c>
       <c r="P20">
-        <v>0.04</v>
+        <v>5.83</v>
       </c>
       <c r="Q20">
-        <v>601.61999999999989</v>
+        <v>3299.2499999999995</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>1717.58</v>
+        <v>867.66</v>
       </c>
       <c r="C21">
-        <v>235.58</v>
+        <v>157.61000000000001</v>
       </c>
       <c r="D21">
-        <v>594.42999999999995</v>
+        <v>116.84</v>
       </c>
       <c r="E21">
-        <v>489.34</v>
+        <v>169.15</v>
       </c>
       <c r="F21">
-        <v>86.34</v>
+        <v>33.130000000000003</v>
       </c>
       <c r="G21">
-        <v>54.83</v>
+        <v>26.74</v>
       </c>
       <c r="H21">
-        <v>93.74</v>
+        <v>19.57</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>77.12</v>
       </c>
       <c r="J21">
-        <v>0.63</v>
+        <v>5.04</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
+        <v>20.41</v>
+      </c>
+      <c r="M21">
+        <v>1.55</v>
+      </c>
+      <c r="N21">
         <v>0</v>
       </c>
-      <c r="M21">
-        <v>10.87</v>
-      </c>
-      <c r="N21">
-        <v>9.61</v>
-      </c>
       <c r="O21">
-        <v>0.47</v>
+        <v>0.39</v>
       </c>
       <c r="P21">
-        <v>5.83</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <v>3299.2499999999995</v>
+        <v>1495.21</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22">
-        <v>867.66</v>
+        <v>1052.96</v>
       </c>
       <c r="C22">
-        <v>157.61000000000001</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>116.84</v>
+        <v>66.040000000000006</v>
       </c>
       <c r="E22">
-        <v>169.15</v>
+        <v>211.81</v>
       </c>
       <c r="F22">
-        <v>33.130000000000003</v>
+        <v>26.15</v>
       </c>
       <c r="G22">
-        <v>26.74</v>
+        <v>26.12</v>
       </c>
       <c r="H22">
-        <v>19.57</v>
+        <v>31.76</v>
       </c>
       <c r="I22">
-        <v>77.12</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>5.04</v>
+        <v>30.07</v>
       </c>
       <c r="K22">
+        <v>2.6</v>
+      </c>
+      <c r="L22">
+        <v>10.75</v>
+      </c>
+      <c r="M22">
         <v>0</v>
-      </c>
-      <c r="L22">
-        <v>20.41</v>
-      </c>
-      <c r="M22">
-        <v>1.55</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
       <c r="O22">
-        <v>0.39</v>
+        <v>0.72</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="Q22">
-        <v>1495.21</v>
+        <v>1461.5800000000002</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>1052.96</v>
+        <v>287.32</v>
       </c>
       <c r="C23">
+        <v>364.05</v>
+      </c>
+      <c r="D23">
+        <v>183.99</v>
+      </c>
+      <c r="E23">
+        <v>194.17</v>
+      </c>
+      <c r="F23">
+        <v>12.72</v>
+      </c>
+      <c r="G23">
+        <v>8.49</v>
+      </c>
+      <c r="H23">
+        <v>12.88</v>
+      </c>
+      <c r="I23">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="J23">
+        <v>16.14</v>
+      </c>
+      <c r="K23">
+        <v>15.01</v>
+      </c>
+      <c r="L23">
+        <v>1.71</v>
+      </c>
+      <c r="M23">
+        <v>0.83</v>
+      </c>
+      <c r="N23">
+        <v>2.37</v>
+      </c>
+      <c r="O23">
+        <v>0.7</v>
+      </c>
+      <c r="P23">
         <v>0</v>
       </c>
-      <c r="D23">
-        <v>66.040000000000006</v>
-      </c>
-      <c r="E23">
-        <v>211.81</v>
-      </c>
-      <c r="F23">
-        <v>26.15</v>
-      </c>
-      <c r="G23">
-        <v>26.12</v>
-      </c>
-      <c r="H23">
-        <v>31.76</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>30.07</v>
-      </c>
-      <c r="K23">
-        <v>2.6</v>
-      </c>
-      <c r="L23">
-        <v>10.75</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0.72</v>
-      </c>
-      <c r="P23">
-        <v>2.6</v>
-      </c>
       <c r="Q23">
-        <v>1461.5800000000002</v>
+        <v>1116.69</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24">
-        <v>287.32</v>
+        <v>621.02</v>
       </c>
       <c r="C24">
-        <v>364.05</v>
+        <v>359.4</v>
       </c>
       <c r="D24">
-        <v>183.99</v>
+        <v>43.12</v>
       </c>
       <c r="E24">
-        <v>194.17</v>
+        <v>159.31</v>
       </c>
       <c r="F24">
-        <v>12.72</v>
+        <v>6.11</v>
       </c>
       <c r="G24">
-        <v>8.49</v>
+        <v>26.4</v>
       </c>
       <c r="H24">
-        <v>12.88</v>
+        <v>76.650000000000006</v>
       </c>
       <c r="I24">
-        <v>16.309999999999999</v>
+        <v>14.53</v>
       </c>
       <c r="J24">
-        <v>16.14</v>
+        <v>2.06</v>
       </c>
       <c r="K24">
-        <v>15.01</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>1.71</v>
+        <v>0.46</v>
       </c>
       <c r="M24">
-        <v>0.83</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <v>2.37</v>
+        <v>0.03</v>
       </c>
       <c r="O24">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="Q24">
-        <v>1116.69</v>
+        <v>1312.11</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25">
-        <v>621.02</v>
+        <v>471.44</v>
       </c>
       <c r="C25">
-        <v>359.4</v>
+        <v>58.06</v>
       </c>
       <c r="D25">
-        <v>43.12</v>
+        <v>40.72</v>
       </c>
       <c r="E25">
-        <v>159.31</v>
+        <v>135.49</v>
       </c>
       <c r="F25">
-        <v>6.11</v>
+        <v>0.95</v>
       </c>
       <c r="G25">
-        <v>26.4</v>
+        <v>12.21</v>
       </c>
       <c r="H25">
-        <v>76.650000000000006</v>
+        <v>17.77</v>
       </c>
       <c r="I25">
-        <v>14.53</v>
+        <v>7.82</v>
       </c>
       <c r="J25">
-        <v>2.06</v>
+        <v>20.92</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L25">
-        <v>0.46</v>
+        <v>1.24</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>1.56</v>
       </c>
       <c r="N25">
-        <v>0.03</v>
+        <v>3.07</v>
       </c>
       <c r="O25">
-        <v>0.8</v>
+        <v>0.99</v>
       </c>
       <c r="P25">
-        <v>2.2200000000000002</v>
+        <v>1.97</v>
       </c>
       <c r="Q25">
-        <v>1312.11</v>
+        <v>779.21</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>471.44</v>
+        <v>179.48</v>
       </c>
       <c r="C26">
-        <v>58.06</v>
+        <v>36.35</v>
       </c>
       <c r="D26">
-        <v>40.72</v>
+        <v>33.08</v>
       </c>
       <c r="E26">
-        <v>135.49</v>
+        <v>59.47</v>
       </c>
       <c r="F26">
-        <v>0.95</v>
+        <v>20.72</v>
       </c>
       <c r="G26">
-        <v>12.21</v>
+        <v>10.82</v>
       </c>
       <c r="H26">
-        <v>17.77</v>
+        <v>5.29</v>
       </c>
       <c r="I26">
-        <v>7.82</v>
+        <v>1.32</v>
       </c>
       <c r="J26">
-        <v>20.92</v>
+        <v>3.41</v>
       </c>
       <c r="K26">
-        <v>5</v>
+        <v>0.31</v>
       </c>
       <c r="L26">
-        <v>1.24</v>
+        <v>1.41</v>
       </c>
       <c r="M26">
-        <v>1.56</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>3.07</v>
+        <v>0.26</v>
       </c>
       <c r="O26">
-        <v>0.99</v>
+        <v>1.01</v>
       </c>
       <c r="P26">
-        <v>1.97</v>
+        <v>1.01</v>
       </c>
       <c r="Q26">
-        <v>779.21</v>
+        <v>353.93999999999994</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>179.48</v>
+        <v>634.76</v>
       </c>
       <c r="C27">
-        <v>36.35</v>
+        <v>161.22</v>
       </c>
       <c r="D27">
-        <v>33.08</v>
+        <v>61.31</v>
       </c>
       <c r="E27">
-        <v>59.47</v>
+        <v>224.9</v>
       </c>
       <c r="F27">
-        <v>20.72</v>
+        <v>56.14</v>
       </c>
       <c r="G27">
-        <v>10.82</v>
+        <v>21.2</v>
       </c>
       <c r="H27">
-        <v>5.29</v>
+        <v>10.53</v>
       </c>
       <c r="I27">
-        <v>1.32</v>
+        <v>7.92</v>
       </c>
       <c r="J27">
-        <v>3.41</v>
+        <v>11.38</v>
       </c>
       <c r="K27">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="L27">
-        <v>1.41</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>1.04</v>
       </c>
       <c r="N27">
-        <v>0.26</v>
+        <v>0.19</v>
       </c>
       <c r="O27">
-        <v>1.01</v>
+        <v>0.43</v>
       </c>
       <c r="P27">
-        <v>1.01</v>
+        <v>0.19</v>
       </c>
       <c r="Q27">
-        <v>353.93999999999994</v>
+        <v>1191.21</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B28">
-        <v>634.76</v>
+        <v>262.25</v>
       </c>
       <c r="C28">
-        <v>161.22</v>
+        <v>761.74</v>
       </c>
       <c r="D28">
-        <v>61.31</v>
+        <v>38.64</v>
       </c>
       <c r="E28">
-        <v>224.9</v>
+        <v>222.1</v>
       </c>
       <c r="F28">
-        <v>56.14</v>
+        <v>42.73</v>
       </c>
       <c r="G28">
-        <v>21.2</v>
+        <v>31.47</v>
       </c>
       <c r="H28">
-        <v>10.53</v>
+        <v>111.97</v>
       </c>
       <c r="I28">
-        <v>7.92</v>
+        <v>15.78</v>
       </c>
       <c r="J28">
-        <v>11.38</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>3.94</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="M28">
-        <v>1.04</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="N28">
-        <v>0.19</v>
+        <v>3.52</v>
       </c>
       <c r="O28">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="P28">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="Q28">
-        <v>1191.21</v>
+        <v>1499.96</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>2784.26</v>
+      </c>
+      <c r="C29">
+        <v>2701.06</v>
+      </c>
+      <c r="D29">
+        <v>1158.3900000000001</v>
+      </c>
+      <c r="E29">
+        <v>703.48</v>
+      </c>
+      <c r="F29">
+        <v>46.37</v>
+      </c>
+      <c r="G29">
+        <v>217.72</v>
+      </c>
+      <c r="H29">
+        <v>70.34</v>
+      </c>
+      <c r="I29">
+        <v>111.43</v>
+      </c>
+      <c r="J29">
+        <v>205.03</v>
+      </c>
+      <c r="K29">
+        <v>59.75</v>
+      </c>
+      <c r="L29">
+        <v>90.08</v>
+      </c>
+      <c r="M29">
+        <v>9.57</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>8158.5700000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f>SUM(B3:B29)</f>
+        <v>23532.449999999997</v>
+      </c>
+      <c r="C30">
+        <f>SUM(C3:C29)</f>
+        <v>10656.269999999999</v>
+      </c>
+      <c r="D30">
+        <f>SUM(D3:D29)</f>
+        <v>6577.7200000000012</v>
+      </c>
+      <c r="E30">
+        <f>SUM(E3:E29)</f>
+        <v>5841.1400000000012</v>
+      </c>
+      <c r="F30">
+        <f>SUM(F3:F29)</f>
+        <v>1966.58</v>
+      </c>
+      <c r="G30">
+        <f>SUM(G3:G29)</f>
+        <v>1108.6700000000003</v>
+      </c>
+      <c r="H30">
+        <f>SUM(H3:H29)</f>
+        <v>919.07999999999993</v>
+      </c>
+      <c r="I30">
+        <f>SUM(I3:I29)</f>
+        <v>705.09999999999991</v>
+      </c>
+      <c r="J30">
+        <f>SUM(J3:J29)</f>
+        <v>694.58</v>
+      </c>
+      <c r="K30">
+        <f>SUM(K3:K29)</f>
+        <v>344.53999999999996</v>
+      </c>
+      <c r="L30">
+        <f>SUM(L3:L29)</f>
+        <v>264.44</v>
+      </c>
+      <c r="M30">
+        <f>SUM(M3:M29)</f>
+        <v>63.059999999999995</v>
+      </c>
+      <c r="N30">
+        <f>SUM(N3:N29)</f>
+        <v>34.85</v>
+      </c>
+      <c r="O30">
+        <f>SUM(O3:O29)</f>
+        <v>28.969999999999995</v>
+      </c>
+      <c r="P30">
+        <f>SUM(P3:P29)</f>
+        <v>24.84</v>
+      </c>
+      <c r="Q30">
+        <f>SUM(Q3:Q29)</f>
+        <v>52762.29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" t="s">
+        <v>29</v>
+      </c>
+      <c r="J36" t="s">
+        <v>31</v>
+      </c>
+      <c r="K36" t="s">
+        <v>33</v>
+      </c>
+      <c r="L36" t="s">
+        <v>30</v>
+      </c>
+      <c r="M36" t="s">
+        <v>41</v>
+      </c>
+      <c r="N36" t="s">
+        <v>1</v>
+      </c>
+      <c r="O36" t="s">
+        <v>38</v>
+      </c>
+      <c r="P36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="120">
+        <f>B30/$Q$30</f>
+        <v>0.44600888248027137</v>
+      </c>
+      <c r="C37" s="120">
+        <f>C30/$Q$30</f>
+        <v>0.20196754159078384</v>
+      </c>
+      <c r="D37" s="120">
+        <f>D30/$Q$30</f>
+        <v>0.12466706808972849</v>
+      </c>
+      <c r="E37" s="120">
+        <f>E30/$Q$30</f>
+        <v>0.11070671875690007</v>
+      </c>
+      <c r="F37" s="120">
+        <f>F30/$Q$30</f>
+        <v>3.7272453489035441E-2</v>
+      </c>
+      <c r="G37" s="120">
+        <f>G30/$Q$30</f>
+        <v>2.101254513403418E-2</v>
+      </c>
+      <c r="H37" s="120">
+        <f>H30/$Q$30</f>
+        <v>1.7419259095842882E-2</v>
+      </c>
+      <c r="I37" s="120">
+        <f>I30/$Q$30</f>
+        <v>1.3363711089871192E-2</v>
+      </c>
+      <c r="J37" s="120">
+        <f>J30/$Q$30</f>
+        <v>1.3164326264079896E-2</v>
+      </c>
+      <c r="K37" s="120">
+        <f>K30/$Q$30</f>
+        <v>6.5300425739671262E-3</v>
+      </c>
+      <c r="L37" s="120">
+        <f>L30/$Q$30</f>
+        <v>5.0119128642824255E-3</v>
+      </c>
+      <c r="M37" s="120">
+        <f>M30/$Q$30</f>
+        <v>1.1951717789352963E-3</v>
+      </c>
+      <c r="N37" s="120">
+        <f>N30/$Q$30</f>
+        <v>6.6050961775919882E-4</v>
+      </c>
+      <c r="O37" s="120">
+        <f>O30/$Q$30</f>
+        <v>5.4906638813440425E-4</v>
+      </c>
+      <c r="P37" s="120">
+        <f>P30/$Q$30</f>
+        <v>4.7079078637413195E-4</v>
+      </c>
+      <c r="Q37" s="120">
+        <f>Q30/$Q$30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="119">
+        <f>Q3/$Q$30</f>
+        <v>4.9789916245106119E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="119">
+        <f>Q4/$Q$30</f>
+        <v>7.5832000468516431E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="119">
+        <f>Q5/$Q$30</f>
+        <v>1.101714880078177E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="119">
+        <f>Q6/$Q$30</f>
+        <v>1.6186939573699325E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="119">
+        <f>Q7/$Q$30</f>
+        <v>6.6657455542585434E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="119">
+        <f>Q8/$Q$30</f>
+        <v>1.4287855966827821E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="119">
+        <f>Q9/$Q$30</f>
+        <v>8.2927977538503353E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="119">
+        <f>Q10/$Q$30</f>
+        <v>1.989489083965082E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="119">
+        <f>Q11/$Q$30</f>
+        <v>7.5937568289776658E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="119">
+        <f>Q12/$Q$30</f>
+        <v>7.07054223764738E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="119">
+        <f>Q13/$Q$30</f>
+        <v>5.7175115030071666E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="119">
+        <f>Q14/$Q$30</f>
+        <v>1.6716294914417097E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="119">
+        <f>Q15/$Q$30</f>
+        <v>1.4267007743598695E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="119">
+        <f>Q16/$Q$30</f>
+        <v>3.3253295109063691E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="119">
+        <f>Q17/$Q$30</f>
+        <v>3.6151956255120847E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="119">
+        <f>Q18/$Q$30</f>
+        <v>1.6074359168262026E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="119">
+        <f>Q19/$Q$30</f>
+        <v>1.1402461871916474E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="119">
+        <f>Q20/$Q$30</f>
+        <v>6.2530454989728451E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="119">
+        <f>Q21/$Q$30</f>
+        <v>2.8338610776749835E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="119">
+        <f>Q22/$Q$30</f>
+        <v>2.7701223733844763E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="119">
+        <f>Q23/$Q$30</f>
+        <v>2.1164547634304729E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="119">
+        <f>Q24/$Q$30</f>
+        <v>2.4868329255610395E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="119">
+        <f>Q25/$Q$30</f>
+        <v>1.4768312747608188E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="119">
+        <f>Q26/$Q$30</f>
+        <v>6.7082001179251307E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="119">
+        <f>Q27/$Q$30</f>
+        <v>2.2576919993427123E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>20</v>
       </c>
-      <c r="B29">
-        <v>262.25</v>
-      </c>
-      <c r="C29">
-        <v>761.74</v>
-      </c>
-      <c r="D29">
-        <v>38.64</v>
-      </c>
-      <c r="E29">
-        <v>222.1</v>
-      </c>
-      <c r="F29">
-        <v>42.73</v>
-      </c>
-      <c r="G29">
-        <v>31.47</v>
-      </c>
-      <c r="H29">
-        <v>111.97</v>
-      </c>
-      <c r="I29">
-        <v>15.78</v>
-      </c>
-      <c r="J29">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="K29">
-        <v>3.94</v>
-      </c>
-      <c r="L29">
-        <v>0.65</v>
-      </c>
-      <c r="M29">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="N29">
-        <v>3.52</v>
-      </c>
-      <c r="O29">
-        <v>0.61</v>
-      </c>
-      <c r="P29">
-        <v>0.2</v>
-      </c>
-      <c r="Q29">
-        <v>1499.96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B65" s="119">
+        <f>Q28/$Q$30</f>
+        <v>2.8428637195239252E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>2</v>
       </c>
-      <c r="B30">
-        <v>2784.26</v>
-      </c>
-      <c r="C30">
-        <v>2701.06</v>
-      </c>
-      <c r="D30">
-        <v>1158.3900000000001</v>
-      </c>
-      <c r="E30">
-        <v>703.48</v>
-      </c>
-      <c r="F30">
-        <v>46.37</v>
-      </c>
-      <c r="G30">
-        <v>217.72</v>
-      </c>
-      <c r="H30">
-        <v>70.34</v>
-      </c>
-      <c r="I30">
-        <v>111.43</v>
-      </c>
-      <c r="J30">
-        <v>205.03</v>
-      </c>
-      <c r="K30">
-        <v>59.75</v>
-      </c>
-      <c r="L30">
-        <v>90.08</v>
-      </c>
-      <c r="M30">
-        <v>9.57</v>
-      </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="O30">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>8158.5700000000006</v>
+      <c r="B66" s="119">
+        <f>Q29/$Q$30</f>
+        <v>0.15462880780951699</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="119">
+        <f>Q30/$Q$30</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -31299,8 +31678,8 @@
         <v>88</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>

</xml_diff>